<commit_message>
Refactor CorrectCode and CorrectSentence models: add completed field to CorrectCode and remove from CorrectSentence; update related logic in routes
</commit_message>
<xml_diff>
--- a/init_db.xlsx
+++ b/init_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.sobczyk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_files\My projects\math_days_sp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A9B93E-9F2F-475A-8BA7-4199F969D418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB374C52-84BD-4699-93A1-E17B9ECC6106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{440E4114-BA55-4D18-A151-265229C34578}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{440E4114-BA55-4D18-A151-265229C34578}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="4" r:id="rId1"/>
@@ -328,69 +328,9 @@
     <t>Grawitacja</t>
   </si>
   <si>
-    <t>Europa</t>
-  </si>
-  <si>
-    <t>Azja</t>
-  </si>
-  <si>
-    <t>Ocean Atlantycki</t>
-  </si>
-  <si>
-    <t>Ocean Spokojny</t>
-  </si>
-  <si>
     <t>Sahara</t>
   </si>
   <si>
-    <t>Wielka Brytania</t>
-  </si>
-  <si>
-    <t>Kanada</t>
-  </si>
-  <si>
-    <t>Himalaje</t>
-  </si>
-  <si>
-    <t>Alpy</t>
-  </si>
-  <si>
-    <t>Andy</t>
-  </si>
-  <si>
-    <t>Zwrotnik Raka</t>
-  </si>
-  <si>
-    <t>Hiszpania</t>
-  </si>
-  <si>
-    <t>Lądolód</t>
-  </si>
-  <si>
-    <t>Surowce mineralne</t>
-  </si>
-  <si>
-    <t>Czarnoziemy</t>
-  </si>
-  <si>
-    <t>Dorzecze</t>
-  </si>
-  <si>
-    <t>Klimat</t>
-  </si>
-  <si>
-    <t>Skała macierzysta</t>
-  </si>
-  <si>
-    <t>Krasowienie</t>
-  </si>
-  <si>
-    <t>Wyżyna Śląska</t>
-  </si>
-  <si>
-    <t>Migracje</t>
-  </si>
-  <si>
     <t>+1</t>
   </si>
   <si>
@@ -491,6 +431,66 @@
   </si>
   <si>
     <t>7g</t>
+  </si>
+  <si>
+    <t>Mapa hipsometryczna</t>
+  </si>
+  <si>
+    <t>Poziomica</t>
+  </si>
+  <si>
+    <t>Skala mapy</t>
+  </si>
+  <si>
+    <t>Krajobrazy Ziemi</t>
+  </si>
+  <si>
+    <t>Krainy geograficzne</t>
+  </si>
+  <si>
+    <t>Formy krasowe</t>
+  </si>
+  <si>
+    <t>Jaskinie krasowe</t>
+  </si>
+  <si>
+    <t>Wąwozy lessowe</t>
+  </si>
+  <si>
+    <t>Jeziora polodowcowe</t>
+  </si>
+  <si>
+    <t>Dżungla równikowa</t>
+  </si>
+  <si>
+    <t>Ruch wirowy Ziemi</t>
+  </si>
+  <si>
+    <t>Dzień polarny</t>
+  </si>
+  <si>
+    <t>Wszechświat</t>
+  </si>
+  <si>
+    <t>Układ Słoneczny</t>
+  </si>
+  <si>
+    <t>Droga Mleczna</t>
+  </si>
+  <si>
+    <t>Teoria heliocentryczna</t>
+  </si>
+  <si>
+    <t>Rzeźba polodowcowa</t>
+  </si>
+  <si>
+    <t>Kraj jednonarodowy</t>
+  </si>
+  <si>
+    <t>Rezerwat przyrody</t>
+  </si>
+  <si>
+    <t>Góry młode</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -546,6 +546,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA54561-7CDB-442F-A9B8-5E36862FAF39}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -890,112 +891,112 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1019,22 +1020,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2046,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A295E9C4-6C72-4BF7-B041-2806657780A4}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,13 +2060,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,7 +2077,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2087,7 +2088,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,7 +2099,7 @@
         <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,7 +2110,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,7 +2121,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2132,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2143,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2154,7 @@
         <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2176,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2187,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,7 +2198,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2208,7 +2209,7 @@
         <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,7 +2220,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,7 +2231,7 @@
         <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2242,7 @@
         <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,7 +2253,7 @@
         <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,7 +2264,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2275,7 @@
         <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,7 +2286,7 @@
         <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2297,7 @@
         <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,7 +2308,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2319,7 @@
         <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2330,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2341,7 @@
         <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,7 +2352,7 @@
         <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,7 +2363,7 @@
         <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,7 +2374,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,7 +2385,7 @@
         <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,7 +2396,7 @@
         <v>82</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2406,7 +2407,7 @@
         <v>83</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,7 +2418,7 @@
         <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2429,7 @@
         <v>85</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2439,7 +2440,7 @@
         <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2450,7 +2451,7 @@
         <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2462,7 @@
         <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2472,7 +2473,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2483,7 +2484,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,7 +2495,7 @@
         <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,7 +2506,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,7 +2517,7 @@
         <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,238 +2528,238 @@
         <v>94</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>95</v>
+      <c r="B44" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>96</v>
+      <c r="B45" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>97</v>
+      <c r="B46" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>99</v>
+      <c r="B48" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>100</v>
+      <c r="B49" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>101</v>
+      <c r="B50" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>102</v>
+      <c r="B51" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>103</v>
+      <c r="B52" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>104</v>
+      <c r="B53" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>105</v>
+      <c r="B54" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>106</v>
+      <c r="B55" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>107</v>
+      <c r="B56" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>108</v>
+      <c r="B57" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>109</v>
+      <c r="B58" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>110</v>
+      <c r="B59" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>111</v>
+      <c r="B60" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>112</v>
+      <c r="B61" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>113</v>
+      <c r="B62" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>114</v>
+      <c r="B63" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>115</v>
+      <c r="B64" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>